<commit_message>
Added Base Pages for All module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CC32F6F7-8555-408B-894F-5013C44A2F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D05C848F-DD75-4E20-915F-1C2189308379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17712" windowHeight="14664" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -14,13 +14,36 @@
     <sheet name="Class" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R29"/>
+  <oleSize ref="A1:O29"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>sdetnumpyninja@gmail.com</t>
+  </si>
+  <si>
+    <t>Feb@2025</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,6 +55,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -52,14 +83,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
@@ -397,14 +431,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{61904FCD-2F64-48BD-AC72-3C27C9D86959}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -437,7 +502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734070C0-1B6A-4792-849F-EBC031903E15}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added addon Feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{09B79508-22F2-466D-8D91-CC80F3DBB920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7D3CBFCA-CCD9-4B39-8BB8-5CB99276125D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Logout</t>
+  </si>
+  <si>
+    <t>LMS</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,6 +507,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Dashboard Addon feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7D3CBFCA-CCD9-4B39-8BB8-5CB99276125D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D3A8D-4D45-46C7-965D-DFABA887A285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="Class" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>username</t>
   </si>
@@ -42,9 +41,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>popup</t>
-  </si>
-  <si>
     <t>menu</t>
   </si>
   <si>
@@ -64,6 +60,51 @@
   </si>
   <si>
     <t>LMS</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>Manage Program</t>
+  </si>
+  <si>
+    <t>Manage User</t>
+  </si>
+  <si>
+    <t>Manage Batch</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Batches</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>Staff Data</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -458,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +513,7 @@
     <col min="4" max="4" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,10 +530,16 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -502,31 +549,67 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
         <v>11</v>
       </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F6" t="s">
-        <v>13</v>
+      <c r="G6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional scenario Dashboard executed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E839DBC3-B2B2-4773-BAC1-C0F66E6E5765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{27BA8E87-001B-4DFB-BDAF-7CBAD7E75E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -14,11 +14,12 @@
     <sheet name="Class" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:O29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -35,9 +36,6 @@
     <t>Feb@2025</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>LMS - Learning Management System</t>
   </si>
   <si>
@@ -75,6 +73,57 @@
   </si>
   <si>
     <t>Edit / Delete</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Staff Data</t>
+  </si>
+  <si>
+    <t>Manage User</t>
+  </si>
+  <si>
+    <t>LMS</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Manage Batch</t>
+  </si>
+  <si>
+    <t>Batches</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -126,7 +175,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
@@ -149,9 +199,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -189,9 +239,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +274,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,9 +326,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,40 +519,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.1328125" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -482,83 +660,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5673E90-C4D8-4E19-B448-4406659E4150}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.265625" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="19.73046875" customWidth="1"/>
-    <col min="5" max="5" width="19.265625" customWidth="1"/>
-    <col min="6" max="6" width="16.73046875" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -572,7 +750,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -586,7 +764,7 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created Program Feature file Addon
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{27BA8E87-001B-4DFB-BDAF-7CBAD7E75E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{29B05389-44AE-4FA3-B4BD-BC96B4818C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>username</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>Manage Class</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
   </si>
 </sst>
 </file>
@@ -521,7 +527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -632,7 +640,9 @@
       <c r="G5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -646,7 +656,9 @@
       <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Executed additional program scn
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,23 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{29B05389-44AE-4FA3-B4BD-BC96B4818C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BD2F6334-B606-41EC-824B-EB5199CCA327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="17928" windowHeight="14664" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
     <sheet name="Program" sheetId="9" r:id="rId2"/>
     <sheet name="Batch" sheetId="10" r:id="rId3"/>
     <sheet name="Class" sheetId="11" r:id="rId4"/>
+    <sheet name="Msg" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O29"/>
+  <oleSize ref="A1:R29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>username</t>
   </si>
@@ -130,6 +131,69 @@
   </si>
   <si>
     <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Name Empty</t>
+  </si>
+  <si>
+    <t>Program name is required.</t>
+  </si>
+  <si>
+    <t>Desc Empty</t>
+  </si>
+  <si>
+    <t>Description is required.</t>
+  </si>
+  <si>
+    <t>Status Empty</t>
+  </si>
+  <si>
+    <t>Status is required.</t>
+  </si>
+  <si>
+    <t>Name Spc char</t>
+  </si>
+  <si>
+    <t>This field should start with an alphabet, no special char and min 2 char.</t>
+  </si>
+  <si>
+    <t>Name Strt char</t>
+  </si>
+  <si>
+    <t>Name Strt num</t>
+  </si>
+  <si>
+    <t>Name min char</t>
+  </si>
+  <si>
+    <t>Desc Strt num</t>
+  </si>
+  <si>
+    <t>Desc min char</t>
+  </si>
+  <si>
+    <t>errmsg</t>
+  </si>
+  <si>
+    <t>testscn</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Test#</t>
+  </si>
+  <si>
+    <t>#Test</t>
+  </si>
+  <si>
+    <t>01Test</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>This field should start with an alphabet and min 2 char.</t>
   </si>
 </sst>
 </file>
@@ -148,6 +212,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -527,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -673,7 +738,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D1" sqref="D1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,4 +845,124 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C865A157-B25B-4C67-A287-8F5077C79E99}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Additional Batch Testcase executed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BD2F6334-B606-41EC-824B-EB5199CCA327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CB6A67E8-4404-469D-A3DA-3C268AF0238F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="17928" windowHeight="14664" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="18576" windowHeight="14664" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Msg" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R29"/>
+  <oleSize ref="A1:P18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>username</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>This field should start with an alphabet and min 2 char.</t>
+  </si>
+  <si>
+    <t>This field should start with an alphabet and min 2 character.</t>
+  </si>
+  <si>
+    <t>#des</t>
   </si>
 </sst>
 </file>
@@ -593,7 +599,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,6 +607,10 @@
     <col min="1" max="1" width="24.109375" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -849,10 +859,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C865A157-B25B-4C67-A287-8F5077C79E99}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,6 +972,17 @@
         <v>57</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Additional class Testcase executed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CB6A67E8-4404-469D-A3DA-3C268AF0238F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2EE84997-88C1-4FD8-9D06-A474FBEAD0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="18576" windowHeight="14664" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="18792" windowHeight="14664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Msg" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P18"/>
+  <oleSize ref="A1:M29"/>
 </workbook>
 </file>
 
@@ -598,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -861,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C865A157-B25B-4C67-A287-8F5077C79E99}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Batch addon Step
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelData.xlsx
+++ b/src/test/resources/TestData/ExcelData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C3A4D791-4555-4D28-9655-BB3C734F1B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0D046948-BFEC-4B3E-95B7-F2816005FA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5856" yWindow="4068" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17496" windowHeight="13464" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="12" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Msg" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M29"/>
+  <oleSize ref="A1:P29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>username</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Invalid username and password Please try again</t>
+  </si>
+  <si>
+    <t>Desc Strt Spl</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A01634-65B9-471D-B1E1-B2B81A92F07E}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -891,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C865A157-B25B-4C67-A287-8F5077C79E99}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,7 +1007,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>59</v>

</xml_diff>